<commit_message>
updated risk management table
</commit_message>
<xml_diff>
--- a/docs/RiskManagement/RiskAnalysisMCMessenger.xlsx
+++ b/docs/RiskManagement/RiskAnalysisMCMessenger.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\se_mcm\docs\RiskManagement\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC4FF5D0-95E3-464F-8729-210DE50FC4FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55D28C0E-351B-4355-AF39-478B439C828F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{2F3C69F8-44BB-0C40-BCA3-734B6A6A670F}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{2F3C69F8-44BB-0C40-BCA3-734B6A6A670F}"/>
   </bookViews>
   <sheets>
     <sheet name="MCM" sheetId="2" r:id="rId1"/>
@@ -220,12 +220,6 @@
     <t>Code injection (security)</t>
   </si>
   <si>
-    <t>Hardware unavailable</t>
-  </si>
-  <si>
-    <t>Hardware resources</t>
-  </si>
-  <si>
     <t>Impact: 1 - 10</t>
   </si>
   <si>
@@ -241,9 +235,6 @@
     <t>Shutdown service, notify developers, restore pre attack version and release hotfix</t>
   </si>
   <si>
-    <t>Strategies for a diversity of the platform (Different devices)</t>
-  </si>
-  <si>
     <t>Chip-Shortage, hardware eol (end of life)</t>
   </si>
   <si>
@@ -292,10 +283,19 @@
     <t>Hope, cry, learn hard, good documentation, cry more</t>
   </si>
   <si>
-    <t>Prof. Dr. Vollmer (Compiler-King)</t>
-  </si>
-  <si>
     <t>cry; try to understand the documentation</t>
+  </si>
+  <si>
+    <t>Project owner</t>
+  </si>
+  <si>
+    <t>Hardware (MC) unavailable</t>
+  </si>
+  <si>
+    <t>Hardware resources (RAM, CPU)</t>
+  </si>
+  <si>
+    <t>Strategies for a diversity of the platform (Different devices). Increase the budget and save some MCs in storage.</t>
   </si>
 </sst>
 </file>
@@ -569,7 +569,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -619,9 +619,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -643,9 +640,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -674,9 +668,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="3" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -998,115 +989,115 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B25F1F0C-8D61-499F-A28C-7939C69BB561}">
   <dimension ref="A1:T22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" zoomScale="84" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.3984375" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15" style="1" customWidth="1"/>
-    <col min="3" max="3" width="21.625" style="5" customWidth="1"/>
-    <col min="4" max="4" width="10.125" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.59765625" style="5" customWidth="1"/>
+    <col min="4" max="4" width="10.09765625" style="5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7.5" style="5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.5" style="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.25" style="5" customWidth="1"/>
-    <col min="8" max="8" width="17.625" style="5" customWidth="1"/>
-    <col min="9" max="9" width="16.25" style="5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.875" style="5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6.875" style="5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.125" style="5" customWidth="1"/>
+    <col min="7" max="7" width="15.19921875" style="5" customWidth="1"/>
+    <col min="8" max="8" width="17.59765625" style="5" customWidth="1"/>
+    <col min="9" max="9" width="16.19921875" style="5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.8984375" style="5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.8984375" style="5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.09765625" style="5" customWidth="1"/>
     <col min="13" max="20" width="11" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="27" t="s">
+    <row r="1" spans="1:14" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="28" t="s">
+      <c r="B1" s="26" t="s">
         <v>41</v>
       </c>
-      <c r="C1" s="29" t="s">
+      <c r="C1" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="29" t="s">
+      <c r="D1" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="29" t="s">
+      <c r="E1" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="29" t="s">
+      <c r="F1" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="29" t="s">
+      <c r="G1" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="H1" s="29" t="s">
+      <c r="H1" s="27" t="s">
         <v>47</v>
       </c>
-      <c r="I1" s="29" t="s">
+      <c r="I1" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="J1" s="29" t="s">
+      <c r="J1" s="27" t="s">
         <v>48</v>
       </c>
-      <c r="K1" s="29" t="s">
+      <c r="K1" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="L1" s="30" t="s">
+      <c r="L1" s="28" t="s">
         <v>14</v>
       </c>
       <c r="N1" s="2"/>
     </row>
-    <row r="2" spans="1:14" ht="54" x14ac:dyDescent="0.25">
-      <c r="A2" s="22">
+    <row r="2" spans="1:14" ht="55.2" x14ac:dyDescent="0.3">
+      <c r="A2" s="21">
         <v>1</v>
       </c>
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="22" t="s">
         <v>43</v>
       </c>
-      <c r="C2" s="24" t="s">
+      <c r="C2" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="24">
+      <c r="D2" s="23">
         <v>3</v>
       </c>
-      <c r="E2" s="24">
+      <c r="E2" s="23">
         <v>10</v>
       </c>
-      <c r="F2" s="25">
+      <c r="F2" s="23">
         <f>D2*E2</f>
         <v>30</v>
       </c>
-      <c r="G2" s="26" t="s">
-        <v>83</v>
-      </c>
-      <c r="H2" s="26" t="s">
+      <c r="G2" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="H2" s="24" t="s">
+        <v>79</v>
+      </c>
+      <c r="I2" s="24" t="s">
+        <v>81</v>
+      </c>
+      <c r="J2" s="24" t="s">
         <v>82</v>
       </c>
-      <c r="I2" s="26" t="s">
-        <v>85</v>
-      </c>
-      <c r="J2" s="26" t="s">
-        <v>84</v>
-      </c>
-      <c r="K2" s="24" t="s">
+      <c r="K2" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="L2" s="31">
+      <c r="L2" s="29">
         <v>45029</v>
       </c>
       <c r="N2" s="4"/>
     </row>
-    <row r="3" spans="1:14" ht="40.5" x14ac:dyDescent="0.25">
-      <c r="A3" s="20">
+    <row r="3" spans="1:14" ht="41.4" x14ac:dyDescent="0.3">
+      <c r="A3" s="19">
         <v>2</v>
       </c>
-      <c r="B3" s="19" t="s">
+      <c r="B3" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="C3" s="18" t="s">
-        <v>77</v>
+      <c r="C3" s="17" t="s">
+        <v>74</v>
       </c>
       <c r="D3" s="16">
         <v>1</v>
@@ -1114,39 +1105,39 @@
       <c r="E3" s="16">
         <v>4</v>
       </c>
-      <c r="F3" s="17">
+      <c r="F3" s="16">
         <f t="shared" ref="F3:F7" si="0">D3*E3</f>
         <v>4</v>
       </c>
-      <c r="G3" s="18" t="s">
+      <c r="G3" s="17" t="s">
+        <v>75</v>
+      </c>
+      <c r="H3" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="I3" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="J3" s="17" t="s">
         <v>78</v>
-      </c>
-      <c r="H3" s="18" t="s">
-        <v>79</v>
-      </c>
-      <c r="I3" s="18" t="s">
-        <v>80</v>
-      </c>
-      <c r="J3" s="18" t="s">
-        <v>81</v>
       </c>
       <c r="K3" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="L3" s="32">
+      <c r="L3" s="30">
         <v>45029</v>
       </c>
       <c r="N3" s="4"/>
     </row>
-    <row r="4" spans="1:14" ht="40.5" x14ac:dyDescent="0.25">
-      <c r="A4" s="20">
+    <row r="4" spans="1:14" ht="41.4" x14ac:dyDescent="0.3">
+      <c r="A4" s="19">
         <v>3</v>
       </c>
-      <c r="B4" s="19" t="s">
+      <c r="B4" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="C4" s="18" t="s">
-        <v>73</v>
+      <c r="C4" s="17" t="s">
+        <v>70</v>
       </c>
       <c r="D4" s="16">
         <v>1</v>
@@ -1154,18 +1145,18 @@
       <c r="E4" s="16">
         <v>6</v>
       </c>
-      <c r="F4" s="17">
+      <c r="F4" s="16">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="G4" s="18" t="s">
-        <v>74</v>
-      </c>
-      <c r="H4" s="18" t="s">
-        <v>76</v>
-      </c>
-      <c r="I4" s="18" t="s">
-        <v>75</v>
+      <c r="G4" s="17" t="s">
+        <v>71</v>
+      </c>
+      <c r="H4" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="I4" s="17" t="s">
+        <v>72</v>
       </c>
       <c r="J4" s="16" t="s">
         <v>18</v>
@@ -1173,19 +1164,19 @@
       <c r="K4" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="L4" s="32">
+      <c r="L4" s="30">
         <v>45029</v>
       </c>
       <c r="N4" s="4"/>
     </row>
-    <row r="5" spans="1:14" ht="67.5" x14ac:dyDescent="0.25">
-      <c r="A5" s="20">
+    <row r="5" spans="1:14" ht="69" x14ac:dyDescent="0.3">
+      <c r="A5" s="19">
         <v>4</v>
       </c>
-      <c r="B5" s="19" t="s">
+      <c r="B5" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="C5" s="18" t="s">
+      <c r="C5" s="17" t="s">
         <v>59</v>
       </c>
       <c r="D5" s="16">
@@ -1194,38 +1185,38 @@
       <c r="E5" s="16">
         <v>10</v>
       </c>
-      <c r="F5" s="17">
+      <c r="F5" s="16">
         <f t="shared" si="0"/>
         <v>40</v>
       </c>
-      <c r="G5" s="18" t="s">
-        <v>65</v>
-      </c>
-      <c r="H5" s="18" t="s">
+      <c r="G5" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="H5" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="I5" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="I5" s="18" t="s">
-        <v>66</v>
-      </c>
-      <c r="J5" s="18" t="s">
+      <c r="J5" s="17" t="s">
         <v>26</v>
       </c>
       <c r="K5" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="L5" s="32">
+      <c r="L5" s="30">
         <v>45029</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="54" x14ac:dyDescent="0.25">
-      <c r="A6" s="20">
+    <row r="6" spans="1:14" ht="110.4" x14ac:dyDescent="0.3">
+      <c r="A6" s="19">
         <v>5</v>
       </c>
-      <c r="B6" s="19" t="s">
+      <c r="B6" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="C6" s="18" t="s">
-        <v>60</v>
+      <c r="C6" s="17" t="s">
+        <v>83</v>
       </c>
       <c r="D6" s="16">
         <v>1</v>
@@ -1233,78 +1224,78 @@
       <c r="E6" s="16">
         <v>10</v>
       </c>
-      <c r="F6" s="17">
+      <c r="F6" s="16">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="G6" s="18" t="s">
-        <v>67</v>
-      </c>
-      <c r="H6" s="18" t="s">
-        <v>68</v>
-      </c>
-      <c r="I6" s="18" t="s">
-        <v>69</v>
-      </c>
-      <c r="J6" s="18" t="s">
+      <c r="G6" s="17" t="s">
+        <v>85</v>
+      </c>
+      <c r="H6" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="I6" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="J6" s="17" t="s">
         <v>26</v>
       </c>
       <c r="K6" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="L6" s="32">
+      <c r="L6" s="30">
         <v>45029</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="68.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="21">
+    <row r="7" spans="1:14" ht="69.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="20">
         <v>6</v>
       </c>
-      <c r="B7" s="33" t="s">
+      <c r="B7" s="31" t="s">
         <v>46</v>
       </c>
-      <c r="C7" s="34" t="s">
-        <v>61</v>
-      </c>
-      <c r="D7" s="35">
+      <c r="C7" s="32" t="s">
+        <v>84</v>
+      </c>
+      <c r="D7" s="33">
         <v>5</v>
       </c>
-      <c r="E7" s="35">
+      <c r="E7" s="33">
         <v>10</v>
       </c>
-      <c r="F7" s="36">
+      <c r="F7" s="33">
         <f t="shared" si="0"/>
         <v>50</v>
       </c>
-      <c r="G7" s="34" t="s">
-        <v>72</v>
-      </c>
-      <c r="H7" s="34" t="s">
-        <v>70</v>
-      </c>
-      <c r="I7" s="34" t="s">
-        <v>71</v>
-      </c>
-      <c r="J7" s="34" t="s">
+      <c r="G7" s="32" t="s">
+        <v>69</v>
+      </c>
+      <c r="H7" s="32" t="s">
+        <v>67</v>
+      </c>
+      <c r="I7" s="32" t="s">
+        <v>68</v>
+      </c>
+      <c r="J7" s="32" t="s">
         <v>26</v>
       </c>
-      <c r="K7" s="35" t="s">
+      <c r="K7" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="L7" s="37">
+      <c r="L7" s="34">
         <v>45029</v>
       </c>
       <c r="N7" s="2"/>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="D8" s="6"/>
       <c r="E8" s="6"/>
       <c r="L8" s="10"/>
       <c r="N8" s="4"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="C9" s="5" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D9" s="6"/>
       <c r="E9" s="6"/>
@@ -1312,9 +1303,9 @@
       <c r="L9" s="10"/>
       <c r="N9" s="4"/>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="C10" s="5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D10" s="6"/>
       <c r="E10" s="6"/>
@@ -1322,7 +1313,7 @@
       <c r="L10" s="10"/>
       <c r="N10" s="4"/>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="C11" s="5" t="s">
         <v>58</v>
       </c>
@@ -1332,63 +1323,63 @@
       <c r="L11" s="10"/>
       <c r="N11" s="4"/>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="D12" s="6"/>
       <c r="E12" s="6"/>
       <c r="I12" s="8"/>
       <c r="L12" s="10"/>
       <c r="N12" s="4"/>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="D13" s="7"/>
       <c r="E13" s="6"/>
       <c r="I13" s="8"/>
       <c r="L13" s="10"/>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="D14" s="7"/>
       <c r="E14" s="6"/>
       <c r="I14" s="8"/>
       <c r="L14" s="10"/>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="D15" s="7"/>
       <c r="E15" s="6"/>
       <c r="I15" s="8"/>
       <c r="L15" s="10"/>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="D16" s="7"/>
       <c r="E16" s="6"/>
       <c r="I16" s="8"/>
       <c r="L16" s="10"/>
       <c r="N16" s="4"/>
     </row>
-    <row r="17" spans="4:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="4:14" x14ac:dyDescent="0.3">
       <c r="D17" s="7"/>
       <c r="I17" s="8"/>
       <c r="L17" s="10"/>
       <c r="N17" s="4"/>
     </row>
-    <row r="18" spans="4:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="4:14" x14ac:dyDescent="0.3">
       <c r="D18" s="7"/>
       <c r="I18" s="8"/>
       <c r="L18" s="10"/>
       <c r="N18" s="4"/>
     </row>
-    <row r="19" spans="4:14" x14ac:dyDescent="0.25">
+    <row r="19" spans="4:14" x14ac:dyDescent="0.3">
       <c r="I19" s="8"/>
       <c r="L19" s="10"/>
       <c r="N19" s="4"/>
     </row>
-    <row r="20" spans="4:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="4:14" x14ac:dyDescent="0.3">
       <c r="L20" s="10"/>
       <c r="N20" s="4"/>
     </row>
-    <row r="21" spans="4:14" x14ac:dyDescent="0.25">
+    <row r="21" spans="4:14" x14ac:dyDescent="0.3">
       <c r="L21" s="10"/>
     </row>
-    <row r="22" spans="4:14" x14ac:dyDescent="0.25">
+    <row r="22" spans="4:14" x14ac:dyDescent="0.3">
       <c r="L22" s="10"/>
     </row>
   </sheetData>
@@ -1427,24 +1418,24 @@
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.3984375" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15" style="1" customWidth="1"/>
     <col min="3" max="3" width="29.5" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.625" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.59765625" style="5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7.5" style="5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.5" style="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="27.625" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="27.59765625" style="5" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="29" style="5" customWidth="1"/>
-    <col min="9" max="9" width="37.875" style="5" customWidth="1"/>
+    <col min="9" max="9" width="37.8984375" style="5" customWidth="1"/>
     <col min="10" max="10" width="19.5" style="5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6.875" style="5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.125" style="5" customWidth="1"/>
-    <col min="13" max="20" width="10.875" style="1"/>
+    <col min="11" max="11" width="6.8984375" style="5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.09765625" style="5" customWidth="1"/>
+    <col min="13" max="20" width="10.8984375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
@@ -1483,7 +1474,7 @@
       </c>
       <c r="N1" s="2"/>
     </row>
-    <row r="2" spans="1:14" ht="54" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A2" s="11">
         <v>1</v>
       </c>
@@ -1523,7 +1514,7 @@
       </c>
       <c r="N2" s="4"/>
     </row>
-    <row r="3" spans="1:14" ht="54" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A3" s="11">
         <v>2</v>
       </c>
@@ -1563,7 +1554,7 @@
       </c>
       <c r="N3" s="4"/>
     </row>
-    <row r="4" spans="1:14" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" ht="69" x14ac:dyDescent="0.3">
       <c r="A4" s="11">
         <v>3</v>
       </c>
@@ -1603,7 +1594,7 @@
       </c>
       <c r="N4" s="4"/>
     </row>
-    <row r="5" spans="1:14" ht="54" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A5" s="11">
         <v>4</v>
       </c>
@@ -1643,7 +1634,7 @@
       </c>
       <c r="N5" s="4"/>
     </row>
-    <row r="6" spans="1:14" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" ht="69" x14ac:dyDescent="0.3">
       <c r="A6" s="11">
         <v>5</v>
       </c>
@@ -1683,7 +1674,7 @@
       </c>
       <c r="N6" s="4"/>
     </row>
-    <row r="7" spans="1:14" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" ht="69" x14ac:dyDescent="0.3">
       <c r="A7" s="11">
         <v>6</v>
       </c>
@@ -1723,7 +1714,7 @@
       </c>
       <c r="M7" s="9"/>
     </row>
-    <row r="8" spans="1:14" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" ht="69" x14ac:dyDescent="0.3">
       <c r="A8" s="11">
         <v>7</v>
       </c>
@@ -1762,7 +1753,7 @@
         <v>45022</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="81" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" ht="82.8" x14ac:dyDescent="0.3">
       <c r="A9" s="11">
         <v>8</v>
       </c>
@@ -1801,7 +1792,7 @@
         <v>45018</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" s="11"/>
       <c r="B10" s="11"/>
       <c r="C10" s="9"/>
@@ -1816,90 +1807,90 @@
       <c r="L10" s="10"/>
       <c r="N10" s="2"/>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="D11" s="6"/>
       <c r="E11" s="6"/>
       <c r="L11" s="10"/>
       <c r="N11" s="4"/>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="D12" s="6"/>
       <c r="E12" s="6"/>
       <c r="I12" s="8"/>
       <c r="L12" s="10"/>
       <c r="N12" s="4"/>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="D13" s="6"/>
       <c r="E13" s="6"/>
       <c r="I13" s="8"/>
       <c r="L13" s="10"/>
       <c r="N13" s="4"/>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="D14" s="6"/>
       <c r="E14" s="6"/>
       <c r="I14" s="8"/>
       <c r="L14" s="10"/>
       <c r="N14" s="4"/>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="D15" s="6"/>
       <c r="E15" s="6"/>
       <c r="I15" s="8"/>
       <c r="L15" s="10"/>
       <c r="N15" s="4"/>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="D16" s="7"/>
       <c r="E16" s="6"/>
       <c r="I16" s="8"/>
       <c r="L16" s="10"/>
     </row>
-    <row r="17" spans="4:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="4:14" x14ac:dyDescent="0.3">
       <c r="D17" s="7"/>
       <c r="E17" s="6"/>
       <c r="I17" s="8"/>
       <c r="L17" s="10"/>
     </row>
-    <row r="18" spans="4:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="4:14" x14ac:dyDescent="0.3">
       <c r="D18" s="7"/>
       <c r="E18" s="6"/>
       <c r="I18" s="8"/>
       <c r="L18" s="10"/>
     </row>
-    <row r="19" spans="4:14" x14ac:dyDescent="0.25">
+    <row r="19" spans="4:14" x14ac:dyDescent="0.3">
       <c r="D19" s="7"/>
       <c r="E19" s="6"/>
       <c r="I19" s="8"/>
       <c r="L19" s="10"/>
       <c r="N19" s="4"/>
     </row>
-    <row r="20" spans="4:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="4:14" x14ac:dyDescent="0.3">
       <c r="D20" s="7"/>
       <c r="I20" s="8"/>
       <c r="L20" s="10"/>
       <c r="N20" s="4"/>
     </row>
-    <row r="21" spans="4:14" x14ac:dyDescent="0.25">
+    <row r="21" spans="4:14" x14ac:dyDescent="0.3">
       <c r="D21" s="7"/>
       <c r="I21" s="8"/>
       <c r="L21" s="10"/>
       <c r="N21" s="4"/>
     </row>
-    <row r="22" spans="4:14" x14ac:dyDescent="0.25">
+    <row r="22" spans="4:14" x14ac:dyDescent="0.3">
       <c r="I22" s="8"/>
       <c r="L22" s="10"/>
       <c r="N22" s="4"/>
     </row>
-    <row r="23" spans="4:14" x14ac:dyDescent="0.25">
+    <row r="23" spans="4:14" x14ac:dyDescent="0.3">
       <c r="L23" s="10"/>
       <c r="N23" s="4"/>
     </row>
-    <row r="24" spans="4:14" x14ac:dyDescent="0.25">
+    <row r="24" spans="4:14" x14ac:dyDescent="0.3">
       <c r="L24" s="10"/>
     </row>
-    <row r="25" spans="4:14" x14ac:dyDescent="0.25">
+    <row r="25" spans="4:14" x14ac:dyDescent="0.3">
       <c r="L25" s="10"/>
     </row>
   </sheetData>

</xml_diff>